<commit_message>
Added description for all testcases
</commit_message>
<xml_diff>
--- a/SevenRMart/src/main/java/Resources/TestData.xlsx
+++ b/SevenRMart/src/main/java/Resources/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CB225AB3-D790-472B-83D8-8AD10760F1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EE69C5B1-8004-4900-B4AA-B368AA2584CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="8" xr2:uid="{E10ACDB2-D59E-4F1A-ADCD-D57C4C45D22F}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="DeleteAdminUserPage" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N11"/>
+  <oleSize ref="A1:P14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -790,7 +790,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Utilities folder moved to com.Obsqura.SevenRMart folder
</commit_message>
<xml_diff>
--- a/SevenRMart/src/main/java/Resources/TestData.xlsx
+++ b/SevenRMart/src/main/java/Resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EE69C5B1-8004-4900-B4AA-B368AA2584CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8E07AF8A-0D9D-4A6A-A756-349ED51D8931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="8" xr2:uid="{E10ACDB2-D59E-4F1A-ADCD-D57C4C45D22F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{E10ACDB2-D59E-4F1A-ADCD-D57C4C45D22F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,10 @@
     <sheet name="PushNotificationPage" sheetId="6" r:id="rId6"/>
     <sheet name="CreateExpenseCategoryPage" sheetId="8" r:id="rId7"/>
     <sheet name="CreateSubCategoryPage" sheetId="12" r:id="rId8"/>
-    <sheet name="DeleteAdminUserPage" sheetId="13" r:id="rId9"/>
+    <sheet name="CreateMobileSidebar" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P14"/>
+  <oleSize ref="A1:O23"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>admin</t>
   </si>
@@ -109,9 +109,6 @@
     <t>sub category</t>
   </si>
   <si>
-    <t>username to be deleted</t>
-  </si>
-  <si>
     <t>Washing Machine</t>
   </si>
   <si>
@@ -121,10 +118,10 @@
     <t xml:space="preserve">Latest News </t>
   </si>
   <si>
-    <t>new-client-admin-users-new</t>
-  </si>
-  <si>
-    <t>admin-user-client</t>
+    <t>new-client-admin-users-staff</t>
+  </si>
+  <si>
+    <t>Grocery</t>
   </si>
 </sst>
 </file>
@@ -490,7 +487,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +578,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +604,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -647,7 +644,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -691,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8ACAA41-3596-4BB7-8273-FC42F58AADF7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -742,7 +739,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -777,7 +774,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -786,26 +783,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA115E32-0835-4607-A5C1-A8AA80C45A07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFEC63C-EB66-4B90-9CC6-A0E66C6E11EF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>